<commit_message>
Website Publish Ready and Windows Service change to web service
</commit_message>
<xml_diff>
--- a/CTROReporting/CTROReporting/Templates/Dashboard Expectation Date Check Template.xlsx
+++ b/CTROReporting/CTROReporting/Templates/Dashboard Expectation Date Check Template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7A09AD-C258-4C48-870E-7F13A6F2D9DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20BB9D3-0EB6-47FB-9E66-945BB6EEDC1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>NCIID</t>
   </si>
@@ -31,7 +31,10 @@
     <t>DASHBOARD DATE</t>
   </si>
   <si>
-    <t>REAL DATE</t>
+    <t>SUBMISSION NUMBER</t>
+  </si>
+  <si>
+    <t>Expected Abstraction Completion Date</t>
   </si>
 </sst>
 </file>
@@ -67,7 +70,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -82,11 +85,14 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -100,13 +106,16 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -122,13 +131,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2C6BEAF4-28EA-445B-AEF3-A60933223AA6}" name="Table1" displayName="Table1" ref="A1:D3" totalsRowShown="0" headerRowDxfId="3" dataDxfId="4">
-  <autoFilter ref="A1:D3" xr:uid="{C3BCEA97-44E0-41E7-9E0D-3777522C94A6}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C748D5EA-51FC-4858-AD6A-074234FDFAC6}" name="NCIID" dataDxfId="5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2C6BEAF4-28EA-445B-AEF3-A60933223AA6}" name="Table1" displayName="Table1" ref="A1:E3" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E3" xr:uid="{C3BCEA97-44E0-41E7-9E0D-3777522C94A6}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{C748D5EA-51FC-4858-AD6A-074234FDFAC6}" name="NCIID" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{EF744ABA-7FC7-40F1-B025-5936BCE3120F}" name="SUBMISSION NUMBER" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{7EEC85DF-53A2-4003-BD76-2E792AE4F599}" name="ACCEPTED DATE" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{7F1547D6-F057-4E15-ABE9-7C64E5C3DEA7}" name="DASHBOARD DATE" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{61F75F84-5FCF-4E0D-9443-B55D2735F914}" name="REAL DATE" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{61F75F84-5FCF-4E0D-9443-B55D2735F914}" name="Expected Abstraction Completion Date" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -397,43 +407,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.6328125" customWidth="1"/>
-    <col min="2" max="4" width="25.6328125" style="5" customWidth="1"/>
+    <col min="1" max="2" width="25.6328125" customWidth="1"/>
+    <col min="3" max="4" width="25.6328125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="50.6328125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="4"/>
+      <c r="B2" s="1"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
-      <c r="B3" s="4"/>
+      <c r="B3" s="1"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>